<commit_message>
update next cosmetic and next cosmetic artist
</commit_message>
<xml_diff>
--- a/public/sheets/dunkbin_next_cosmetic_info.xlsx
+++ b/public/sheets/dunkbin_next_cosmetic_info.xlsx
@@ -415,13 +415,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Minneapolis</v>
+        <v>Cirno</v>
       </c>
       <c r="B2">
-        <v>812</v>
+        <v>833</v>
       </c>
       <c r="C2" t="str">
-        <v>ventusol</v>
+        <v>peterce3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>